<commit_message>
added round 1 numbers
</commit_message>
<xml_diff>
--- a/database/seeds/numbers.xlsx
+++ b/database/seeds/numbers.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn/Documents/NUS/Hackers/eusoff/database/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A6CF5C-3AE5-8246-A354-F02F749D40C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCE8AFA-3AD2-9440-8CE8-0641E148E83C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33420" yWindow="1600" windowWidth="28800" windowHeight="16100" xr2:uid="{FC1533EE-1F79-D746-81F8-7CD84BC7FDEF}"/>
+    <workbookView xWindow="12240" yWindow="460" windowWidth="26160" windowHeight="19700" xr2:uid="{FC1533EE-1F79-D746-81F8-7CD84BC7FDEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="7">
   <si>
     <t>id</t>
   </si>
@@ -44,7 +44,16 @@
     <t>updated_at</t>
   </si>
   <si>
-    <t>taken</t>
+    <t>taken_male</t>
+  </si>
+  <si>
+    <t>taken_female</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -80,9 +89,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,18 +406,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8D69E0-4D6D-AD41-9BBB-CAF1F8247A65}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,503 +424,1100 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
+      </c>
+      <c r="D100" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update round 2 bidding
</commit_message>
<xml_diff>
--- a/database/seeds/numbers.xlsx
+++ b/database/seeds/numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn/Documents/NUS/Hackers/eusoff/database/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCE8AFA-3AD2-9440-8CE8-0641E148E83C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D051D9-169B-FF4E-909B-611DC9D0E235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12240" yWindow="460" windowWidth="26160" windowHeight="19700" xr2:uid="{FC1533EE-1F79-D746-81F8-7CD84BC7FDEF}"/>
   </bookViews>
@@ -60,13 +60,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,15 +413,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8D69E0-4D6D-AD41-9BBB-CAF1F8247A65}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:K406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +437,10 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -439,10 +448,12 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -452,19 +463,23 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -472,10 +487,12 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -483,21 +500,25 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -507,19 +528,23 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -527,10 +552,12 @@
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -540,8 +567,10 @@
       <c r="E11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -551,19 +580,23 @@
       <c r="E12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -573,63 +606,75 @@
       <c r="E14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -637,21 +682,25 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -661,19 +710,23 @@
       <c r="E22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -683,8 +736,10 @@
       <c r="E24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -692,10 +747,12 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -705,8 +762,10 @@
       <c r="E26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -716,8 +775,10 @@
       <c r="E27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -725,10 +786,12 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -736,10 +799,12 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -749,30 +814,36 @@
       <c r="E30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -782,8 +853,10 @@
       <c r="E33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -793,8 +866,10 @@
       <c r="E34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -804,8 +879,10 @@
       <c r="E35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -815,8 +892,10 @@
       <c r="E36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -826,8 +905,10 @@
       <c r="E37" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -835,10 +916,12 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -848,8 +931,10 @@
       <c r="E39" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -859,8 +944,10 @@
       <c r="E40" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -870,8 +957,10 @@
       <c r="E41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -879,21 +968,25 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E43" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -903,8 +996,10 @@
       <c r="E44" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -914,8 +1009,10 @@
       <c r="E45" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -923,10 +1020,12 @@
         <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -936,8 +1035,10 @@
       <c r="E47" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -947,8 +1048,10 @@
       <c r="E48" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -958,8 +1061,10 @@
       <c r="E49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -969,8 +1074,10 @@
       <c r="E50" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -980,8 +1087,10 @@
       <c r="E51" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -991,8 +1100,10 @@
       <c r="E52" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1002,8 +1113,10 @@
       <c r="E53" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1013,8 +1126,10 @@
       <c r="E54" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1024,19 +1139,23 @@
       <c r="E55" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1046,8 +1165,10 @@
       <c r="E57" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1057,8 +1178,10 @@
       <c r="E58" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1068,8 +1191,10 @@
       <c r="E59" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1079,8 +1204,10 @@
       <c r="E60" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1090,8 +1217,10 @@
       <c r="E61" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1101,8 +1230,10 @@
       <c r="E62" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1112,8 +1243,10 @@
       <c r="E63" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1123,8 +1256,10 @@
       <c r="E64" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1134,8 +1269,10 @@
       <c r="E65" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1145,8 +1282,10 @@
       <c r="E66" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1156,8 +1295,10 @@
       <c r="E67" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1167,8 +1308,10 @@
       <c r="E68" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1178,8 +1321,10 @@
       <c r="E69" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1189,8 +1334,10 @@
       <c r="E70" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1200,19 +1347,23 @@
       <c r="E71" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E72" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1222,8 +1373,10 @@
       <c r="E73" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1233,8 +1386,10 @@
       <c r="E74" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1244,8 +1399,10 @@
       <c r="E75" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1255,8 +1412,10 @@
       <c r="E76" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1266,8 +1425,10 @@
       <c r="E77" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1277,8 +1438,10 @@
       <c r="E78" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1288,8 +1451,10 @@
       <c r="E79" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1299,8 +1464,10 @@
       <c r="E80" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1310,8 +1477,10 @@
       <c r="E81" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1321,8 +1490,10 @@
       <c r="E82" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1332,8 +1503,10 @@
       <c r="E83" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1343,8 +1516,10 @@
       <c r="E84" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1354,8 +1529,10 @@
       <c r="E85" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1365,8 +1542,10 @@
       <c r="E86" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1376,8 +1555,10 @@
       <c r="E87" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1387,19 +1568,23 @@
       <c r="E88" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E89" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J89" s="1"/>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1409,8 +1594,10 @@
       <c r="E90" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1420,8 +1607,10 @@
       <c r="E91" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1431,8 +1620,10 @@
       <c r="E92" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1442,8 +1633,10 @@
       <c r="E93" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1453,8 +1646,10 @@
       <c r="E94" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1464,8 +1659,10 @@
       <c r="E95" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1473,21 +1670,25 @@
         <v>6</v>
       </c>
       <c r="E96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E97" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -1497,19 +1698,23 @@
       <c r="E98" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="D99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E99" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -1519,6 +1724,1232 @@
       <c r="E100" t="s">
         <v>6</v>
       </c>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+    </row>
+    <row r="113" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+    </row>
+    <row r="114" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+    </row>
+    <row r="115" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+    </row>
+    <row r="116" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+    </row>
+    <row r="117" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+    </row>
+    <row r="118" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+    </row>
+    <row r="119" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+    </row>
+    <row r="120" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+    </row>
+    <row r="121" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+    </row>
+    <row r="122" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+    </row>
+    <row r="123" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+    </row>
+    <row r="124" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+    </row>
+    <row r="125" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+    </row>
+    <row r="126" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+    </row>
+    <row r="127" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J127" s="1"/>
+      <c r="K127" s="1"/>
+    </row>
+    <row r="128" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J128" s="1"/>
+      <c r="K128" s="1"/>
+    </row>
+    <row r="129" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J129" s="1"/>
+      <c r="K129" s="1"/>
+    </row>
+    <row r="130" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J130" s="1"/>
+      <c r="K130" s="1"/>
+    </row>
+    <row r="131" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+    </row>
+    <row r="132" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+    </row>
+    <row r="133" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+    </row>
+    <row r="134" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+    </row>
+    <row r="135" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+    </row>
+    <row r="136" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+    </row>
+    <row r="137" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+    </row>
+    <row r="138" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+    </row>
+    <row r="139" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+    </row>
+    <row r="140" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+    </row>
+    <row r="141" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+    </row>
+    <row r="142" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+    </row>
+    <row r="143" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+    </row>
+    <row r="144" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+    </row>
+    <row r="145" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+    </row>
+    <row r="146" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+    </row>
+    <row r="147" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+    </row>
+    <row r="148" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J148" s="1"/>
+      <c r="K148" s="1"/>
+    </row>
+    <row r="149" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J149" s="1"/>
+      <c r="K149" s="1"/>
+    </row>
+    <row r="150" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+    </row>
+    <row r="151" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+    </row>
+    <row r="152" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+    </row>
+    <row r="153" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+    </row>
+    <row r="154" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+    </row>
+    <row r="155" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+    </row>
+    <row r="156" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+    </row>
+    <row r="157" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+    </row>
+    <row r="158" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+    </row>
+    <row r="159" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+    </row>
+    <row r="160" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+    </row>
+    <row r="161" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+    </row>
+    <row r="162" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J162" s="1"/>
+      <c r="K162" s="1"/>
+    </row>
+    <row r="163" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J163" s="1"/>
+      <c r="K163" s="1"/>
+    </row>
+    <row r="164" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J164" s="1"/>
+      <c r="K164" s="1"/>
+    </row>
+    <row r="165" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J165" s="1"/>
+      <c r="K165" s="1"/>
+    </row>
+    <row r="166" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J166" s="1"/>
+      <c r="K166" s="1"/>
+    </row>
+    <row r="167" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
+    </row>
+    <row r="168" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+    </row>
+    <row r="169" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+    </row>
+    <row r="170" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+    </row>
+    <row r="171" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+    </row>
+    <row r="172" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J172" s="1"/>
+      <c r="K172" s="1"/>
+    </row>
+    <row r="173" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+    </row>
+    <row r="174" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J174" s="1"/>
+      <c r="K174" s="1"/>
+    </row>
+    <row r="175" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+    </row>
+    <row r="176" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+    </row>
+    <row r="177" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J177" s="1"/>
+      <c r="K177" s="1"/>
+    </row>
+    <row r="178" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+    </row>
+    <row r="179" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+    </row>
+    <row r="180" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J180" s="1"/>
+      <c r="K180" s="1"/>
+    </row>
+    <row r="181" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+    </row>
+    <row r="182" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J182" s="1"/>
+      <c r="K182" s="1"/>
+    </row>
+    <row r="183" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J183" s="1"/>
+      <c r="K183" s="1"/>
+    </row>
+    <row r="184" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J184" s="1"/>
+      <c r="K184" s="1"/>
+    </row>
+    <row r="185" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J185" s="1"/>
+      <c r="K185" s="1"/>
+    </row>
+    <row r="186" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J186" s="1"/>
+      <c r="K186" s="1"/>
+    </row>
+    <row r="187" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+    </row>
+    <row r="188" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J188" s="1"/>
+      <c r="K188" s="1"/>
+    </row>
+    <row r="189" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J189" s="1"/>
+      <c r="K189" s="1"/>
+    </row>
+    <row r="190" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J190" s="1"/>
+      <c r="K190" s="1"/>
+    </row>
+    <row r="191" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J191" s="1"/>
+      <c r="K191" s="1"/>
+    </row>
+    <row r="192" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J192" s="1"/>
+      <c r="K192" s="1"/>
+    </row>
+    <row r="193" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J193" s="1"/>
+      <c r="K193" s="1"/>
+    </row>
+    <row r="194" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J194" s="1"/>
+      <c r="K194" s="1"/>
+    </row>
+    <row r="195" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J195" s="1"/>
+      <c r="K195" s="1"/>
+    </row>
+    <row r="196" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J196" s="1"/>
+      <c r="K196" s="1"/>
+    </row>
+    <row r="197" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J197" s="1"/>
+      <c r="K197" s="1"/>
+    </row>
+    <row r="198" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J198" s="1"/>
+      <c r="K198" s="1"/>
+    </row>
+    <row r="199" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J199" s="1"/>
+      <c r="K199" s="1"/>
+    </row>
+    <row r="200" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J200" s="1"/>
+      <c r="K200" s="1"/>
+    </row>
+    <row r="201" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J201" s="1"/>
+      <c r="K201" s="1"/>
+    </row>
+    <row r="202" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J202" s="1"/>
+      <c r="K202" s="1"/>
+    </row>
+    <row r="203" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J203" s="1"/>
+      <c r="K203" s="1"/>
+    </row>
+    <row r="204" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J204" s="1"/>
+      <c r="K204" s="1"/>
+    </row>
+    <row r="205" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J205" s="1"/>
+      <c r="K205" s="1"/>
+    </row>
+    <row r="206" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J206" s="1"/>
+      <c r="K206" s="1"/>
+    </row>
+    <row r="207" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J207" s="1"/>
+      <c r="K207" s="1"/>
+    </row>
+    <row r="208" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J208" s="1"/>
+      <c r="K208" s="1"/>
+    </row>
+    <row r="209" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J209" s="1"/>
+      <c r="K209" s="1"/>
+    </row>
+    <row r="210" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J210" s="1"/>
+      <c r="K210" s="1"/>
+    </row>
+    <row r="211" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J211" s="1"/>
+      <c r="K211" s="1"/>
+    </row>
+    <row r="212" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J212" s="1"/>
+      <c r="K212" s="1"/>
+    </row>
+    <row r="213" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J213" s="1"/>
+      <c r="K213" s="1"/>
+    </row>
+    <row r="214" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J214" s="1"/>
+      <c r="K214" s="1"/>
+    </row>
+    <row r="215" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J215" s="1"/>
+      <c r="K215" s="1"/>
+    </row>
+    <row r="216" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J216" s="1"/>
+      <c r="K216" s="1"/>
+    </row>
+    <row r="217" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J217" s="1"/>
+      <c r="K217" s="1"/>
+    </row>
+    <row r="218" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J218" s="1"/>
+      <c r="K218" s="1"/>
+    </row>
+    <row r="219" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J219" s="1"/>
+      <c r="K219" s="1"/>
+    </row>
+    <row r="220" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J220" s="1"/>
+      <c r="K220" s="1"/>
+    </row>
+    <row r="221" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J221" s="1"/>
+      <c r="K221" s="1"/>
+    </row>
+    <row r="222" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J222" s="1"/>
+      <c r="K222" s="1"/>
+    </row>
+    <row r="223" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J223" s="1"/>
+      <c r="K223" s="1"/>
+    </row>
+    <row r="224" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J224" s="1"/>
+      <c r="K224" s="1"/>
+    </row>
+    <row r="225" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J225" s="1"/>
+      <c r="K225" s="1"/>
+    </row>
+    <row r="226" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J226" s="1"/>
+      <c r="K226" s="1"/>
+    </row>
+    <row r="227" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J227" s="1"/>
+      <c r="K227" s="1"/>
+    </row>
+    <row r="228" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J228" s="1"/>
+      <c r="K228" s="1"/>
+    </row>
+    <row r="229" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J229" s="1"/>
+      <c r="K229" s="1"/>
+    </row>
+    <row r="230" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J230" s="1"/>
+      <c r="K230" s="1"/>
+    </row>
+    <row r="231" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J231" s="1"/>
+      <c r="K231" s="1"/>
+    </row>
+    <row r="232" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J232" s="1"/>
+      <c r="K232" s="1"/>
+    </row>
+    <row r="233" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J233" s="1"/>
+      <c r="K233" s="1"/>
+    </row>
+    <row r="234" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J234" s="1"/>
+      <c r="K234" s="1"/>
+    </row>
+    <row r="235" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J235" s="1"/>
+      <c r="K235" s="1"/>
+    </row>
+    <row r="236" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J236" s="1"/>
+      <c r="K236" s="1"/>
+    </row>
+    <row r="237" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J237" s="1"/>
+      <c r="K237" s="1"/>
+    </row>
+    <row r="238" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J238" s="1"/>
+      <c r="K238" s="1"/>
+    </row>
+    <row r="239" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J239" s="1"/>
+      <c r="K239" s="1"/>
+    </row>
+    <row r="240" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J240" s="1"/>
+      <c r="K240" s="1"/>
+    </row>
+    <row r="241" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J241" s="1"/>
+      <c r="K241" s="1"/>
+    </row>
+    <row r="242" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J242" s="1"/>
+      <c r="K242" s="1"/>
+    </row>
+    <row r="243" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J243" s="1"/>
+      <c r="K243" s="1"/>
+    </row>
+    <row r="244" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J244" s="1"/>
+      <c r="K244" s="1"/>
+    </row>
+    <row r="245" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J245" s="1"/>
+      <c r="K245" s="1"/>
+    </row>
+    <row r="246" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J246" s="1"/>
+      <c r="K246" s="1"/>
+    </row>
+    <row r="247" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J247" s="1"/>
+      <c r="K247" s="1"/>
+    </row>
+    <row r="248" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J248" s="1"/>
+      <c r="K248" s="1"/>
+    </row>
+    <row r="249" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J249" s="1"/>
+      <c r="K249" s="1"/>
+    </row>
+    <row r="250" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J250" s="1"/>
+      <c r="K250" s="1"/>
+    </row>
+    <row r="251" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J251" s="1"/>
+      <c r="K251" s="1"/>
+    </row>
+    <row r="252" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J252" s="1"/>
+      <c r="K252" s="1"/>
+    </row>
+    <row r="253" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J253" s="1"/>
+      <c r="K253" s="1"/>
+    </row>
+    <row r="254" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J254" s="1"/>
+      <c r="K254" s="1"/>
+    </row>
+    <row r="255" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J255" s="1"/>
+      <c r="K255" s="1"/>
+    </row>
+    <row r="256" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J256" s="1"/>
+      <c r="K256" s="1"/>
+    </row>
+    <row r="257" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J257" s="1"/>
+      <c r="K257" s="1"/>
+    </row>
+    <row r="258" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J258" s="1"/>
+      <c r="K258" s="1"/>
+    </row>
+    <row r="259" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J259" s="1"/>
+      <c r="K259" s="1"/>
+    </row>
+    <row r="260" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J260" s="1"/>
+      <c r="K260" s="1"/>
+    </row>
+    <row r="261" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J261" s="1"/>
+      <c r="K261" s="1"/>
+    </row>
+    <row r="262" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J262" s="1"/>
+      <c r="K262" s="1"/>
+    </row>
+    <row r="263" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J263" s="1"/>
+      <c r="K263" s="1"/>
+    </row>
+    <row r="264" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J264" s="1"/>
+      <c r="K264" s="1"/>
+    </row>
+    <row r="265" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J265" s="1"/>
+      <c r="K265" s="1"/>
+    </row>
+    <row r="266" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J266" s="1"/>
+      <c r="K266" s="1"/>
+    </row>
+    <row r="267" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J267" s="1"/>
+      <c r="K267" s="1"/>
+    </row>
+    <row r="268" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J268" s="1"/>
+      <c r="K268" s="1"/>
+    </row>
+    <row r="269" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J269" s="1"/>
+      <c r="K269" s="1"/>
+    </row>
+    <row r="270" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J270" s="1"/>
+      <c r="K270" s="1"/>
+    </row>
+    <row r="271" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J271" s="1"/>
+      <c r="K271" s="1"/>
+    </row>
+    <row r="272" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J272" s="1"/>
+      <c r="K272" s="1"/>
+    </row>
+    <row r="273" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J273" s="1"/>
+      <c r="K273" s="1"/>
+    </row>
+    <row r="274" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J274" s="1"/>
+      <c r="K274" s="1"/>
+    </row>
+    <row r="275" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J275" s="1"/>
+      <c r="K275" s="1"/>
+    </row>
+    <row r="276" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J276" s="1"/>
+      <c r="K276" s="1"/>
+    </row>
+    <row r="277" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J277" s="1"/>
+      <c r="K277" s="1"/>
+    </row>
+    <row r="278" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J278" s="1"/>
+      <c r="K278" s="1"/>
+    </row>
+    <row r="279" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J279" s="1"/>
+      <c r="K279" s="1"/>
+    </row>
+    <row r="280" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J280" s="1"/>
+      <c r="K280" s="1"/>
+    </row>
+    <row r="281" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J281" s="1"/>
+      <c r="K281" s="1"/>
+    </row>
+    <row r="282" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J282" s="1"/>
+      <c r="K282" s="1"/>
+    </row>
+    <row r="283" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J283" s="1"/>
+      <c r="K283" s="1"/>
+    </row>
+    <row r="284" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J284" s="1"/>
+      <c r="K284" s="1"/>
+    </row>
+    <row r="285" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J285" s="1"/>
+      <c r="K285" s="1"/>
+    </row>
+    <row r="286" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J286" s="1"/>
+      <c r="K286" s="1"/>
+    </row>
+    <row r="287" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J287" s="1"/>
+      <c r="K287" s="1"/>
+    </row>
+    <row r="288" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J288" s="1"/>
+      <c r="K288" s="1"/>
+    </row>
+    <row r="289" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J289" s="1"/>
+      <c r="K289" s="1"/>
+    </row>
+    <row r="290" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J290" s="1"/>
+      <c r="K290" s="1"/>
+    </row>
+    <row r="291" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J291" s="1"/>
+      <c r="K291" s="1"/>
+    </row>
+    <row r="292" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J292" s="1"/>
+      <c r="K292" s="1"/>
+    </row>
+    <row r="293" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J293" s="1"/>
+      <c r="K293" s="1"/>
+    </row>
+    <row r="294" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J294" s="1"/>
+      <c r="K294" s="1"/>
+    </row>
+    <row r="295" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J295" s="1"/>
+      <c r="K295" s="1"/>
+    </row>
+    <row r="296" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J296" s="1"/>
+      <c r="K296" s="1"/>
+    </row>
+    <row r="297" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J297" s="1"/>
+      <c r="K297" s="1"/>
+    </row>
+    <row r="298" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J298" s="1"/>
+      <c r="K298" s="1"/>
+    </row>
+    <row r="299" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J299" s="1"/>
+      <c r="K299" s="1"/>
+    </row>
+    <row r="300" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J300" s="1"/>
+      <c r="K300" s="1"/>
+    </row>
+    <row r="301" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J301" s="1"/>
+      <c r="K301" s="1"/>
+    </row>
+    <row r="302" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J302" s="1"/>
+      <c r="K302" s="1"/>
+    </row>
+    <row r="303" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J303" s="1"/>
+      <c r="K303" s="1"/>
+    </row>
+    <row r="304" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J304" s="1"/>
+      <c r="K304" s="1"/>
+    </row>
+    <row r="305" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J305" s="1"/>
+      <c r="K305" s="1"/>
+    </row>
+    <row r="306" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J306" s="1"/>
+      <c r="K306" s="1"/>
+    </row>
+    <row r="307" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J307" s="1"/>
+      <c r="K307" s="1"/>
+    </row>
+    <row r="308" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J308" s="1"/>
+      <c r="K308" s="1"/>
+    </row>
+    <row r="309" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J309" s="1"/>
+      <c r="K309" s="1"/>
+    </row>
+    <row r="310" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J310" s="1"/>
+      <c r="K310" s="1"/>
+    </row>
+    <row r="311" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J311" s="1"/>
+      <c r="K311" s="1"/>
+    </row>
+    <row r="312" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J312" s="1"/>
+      <c r="K312" s="1"/>
+    </row>
+    <row r="313" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J313" s="1"/>
+      <c r="K313" s="1"/>
+    </row>
+    <row r="314" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J314" s="1"/>
+      <c r="K314" s="1"/>
+    </row>
+    <row r="315" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J315" s="1"/>
+      <c r="K315" s="1"/>
+    </row>
+    <row r="316" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J316" s="1"/>
+      <c r="K316" s="1"/>
+    </row>
+    <row r="317" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J317" s="1"/>
+      <c r="K317" s="1"/>
+    </row>
+    <row r="318" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J318" s="1"/>
+      <c r="K318" s="1"/>
+    </row>
+    <row r="319" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J319" s="1"/>
+      <c r="K319" s="1"/>
+    </row>
+    <row r="320" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J320" s="1"/>
+      <c r="K320" s="1"/>
+    </row>
+    <row r="321" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J321" s="1"/>
+      <c r="K321" s="1"/>
+    </row>
+    <row r="322" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J322" s="1"/>
+      <c r="K322" s="1"/>
+    </row>
+    <row r="323" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J323" s="1"/>
+      <c r="K323" s="1"/>
+    </row>
+    <row r="324" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J324" s="1"/>
+      <c r="K324" s="1"/>
+    </row>
+    <row r="325" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J325" s="1"/>
+      <c r="K325" s="1"/>
+    </row>
+    <row r="326" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J326" s="1"/>
+      <c r="K326" s="1"/>
+    </row>
+    <row r="327" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J327" s="1"/>
+      <c r="K327" s="1"/>
+    </row>
+    <row r="328" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J328" s="1"/>
+      <c r="K328" s="1"/>
+    </row>
+    <row r="329" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J329" s="1"/>
+      <c r="K329" s="1"/>
+    </row>
+    <row r="330" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J330" s="1"/>
+      <c r="K330" s="1"/>
+    </row>
+    <row r="331" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J331" s="1"/>
+      <c r="K331" s="1"/>
+    </row>
+    <row r="332" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J332" s="1"/>
+      <c r="K332" s="1"/>
+    </row>
+    <row r="333" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J333" s="1"/>
+      <c r="K333" s="1"/>
+    </row>
+    <row r="334" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J334" s="1"/>
+      <c r="K334" s="1"/>
+    </row>
+    <row r="335" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J335" s="1"/>
+      <c r="K335" s="1"/>
+    </row>
+    <row r="336" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J336" s="1"/>
+      <c r="K336" s="1"/>
+    </row>
+    <row r="337" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J337" s="1"/>
+      <c r="K337" s="1"/>
+    </row>
+    <row r="338" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J338" s="1"/>
+      <c r="K338" s="1"/>
+    </row>
+    <row r="339" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J339" s="1"/>
+      <c r="K339" s="1"/>
+    </row>
+    <row r="340" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J340" s="1"/>
+      <c r="K340" s="1"/>
+    </row>
+    <row r="341" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J341" s="1"/>
+      <c r="K341" s="1"/>
+    </row>
+    <row r="342" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J342" s="1"/>
+      <c r="K342" s="1"/>
+    </row>
+    <row r="343" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J343" s="1"/>
+      <c r="K343" s="1"/>
+    </row>
+    <row r="344" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J344" s="1"/>
+      <c r="K344" s="1"/>
+    </row>
+    <row r="345" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J345" s="1"/>
+      <c r="K345" s="1"/>
+    </row>
+    <row r="346" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J346" s="1"/>
+      <c r="K346" s="1"/>
+    </row>
+    <row r="347" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J347" s="1"/>
+      <c r="K347" s="1"/>
+    </row>
+    <row r="348" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J348" s="1"/>
+      <c r="K348" s="1"/>
+    </row>
+    <row r="349" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J349" s="1"/>
+      <c r="K349" s="1"/>
+    </row>
+    <row r="350" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J350" s="1"/>
+      <c r="K350" s="1"/>
+    </row>
+    <row r="351" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J351" s="1"/>
+      <c r="K351" s="1"/>
+    </row>
+    <row r="352" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J352" s="1"/>
+      <c r="K352" s="1"/>
+    </row>
+    <row r="353" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J353" s="1"/>
+      <c r="K353" s="1"/>
+    </row>
+    <row r="354" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J354" s="1"/>
+      <c r="K354" s="1"/>
+    </row>
+    <row r="355" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J355" s="1"/>
+      <c r="K355" s="1"/>
+    </row>
+    <row r="356" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J356" s="1"/>
+      <c r="K356" s="1"/>
+    </row>
+    <row r="357" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J357" s="1"/>
+      <c r="K357" s="1"/>
+    </row>
+    <row r="358" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J358" s="1"/>
+      <c r="K358" s="1"/>
+    </row>
+    <row r="359" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J359" s="1"/>
+      <c r="K359" s="1"/>
+    </row>
+    <row r="360" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J360" s="1"/>
+      <c r="K360" s="1"/>
+    </row>
+    <row r="361" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J361" s="1"/>
+      <c r="K361" s="1"/>
+    </row>
+    <row r="362" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J362" s="1"/>
+      <c r="K362" s="1"/>
+    </row>
+    <row r="363" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J363" s="1"/>
+      <c r="K363" s="1"/>
+    </row>
+    <row r="364" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J364" s="1"/>
+      <c r="K364" s="1"/>
+    </row>
+    <row r="365" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J365" s="1"/>
+      <c r="K365" s="1"/>
+    </row>
+    <row r="366" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J366" s="1"/>
+      <c r="K366" s="1"/>
+    </row>
+    <row r="367" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J367" s="1"/>
+      <c r="K367" s="1"/>
+    </row>
+    <row r="368" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J368" s="1"/>
+      <c r="K368" s="1"/>
+    </row>
+    <row r="369" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J369" s="1"/>
+      <c r="K369" s="1"/>
+    </row>
+    <row r="370" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J370" s="1"/>
+      <c r="K370" s="1"/>
+    </row>
+    <row r="371" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J371" s="1"/>
+      <c r="K371" s="1"/>
+    </row>
+    <row r="372" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J372" s="1"/>
+      <c r="K372" s="1"/>
+    </row>
+    <row r="373" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J373" s="1"/>
+      <c r="K373" s="1"/>
+    </row>
+    <row r="374" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J374" s="1"/>
+      <c r="K374" s="1"/>
+    </row>
+    <row r="375" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J375" s="1"/>
+      <c r="K375" s="1"/>
+    </row>
+    <row r="376" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J376" s="1"/>
+      <c r="K376" s="1"/>
+    </row>
+    <row r="377" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J377" s="1"/>
+      <c r="K377" s="1"/>
+    </row>
+    <row r="378" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J378" s="1"/>
+      <c r="K378" s="1"/>
+    </row>
+    <row r="379" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J379" s="1"/>
+      <c r="K379" s="1"/>
+    </row>
+    <row r="380" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J380" s="1"/>
+      <c r="K380" s="1"/>
+    </row>
+    <row r="381" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J381" s="1"/>
+      <c r="K381" s="1"/>
+    </row>
+    <row r="382" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J382" s="1"/>
+      <c r="K382" s="1"/>
+    </row>
+    <row r="383" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J383" s="1"/>
+      <c r="K383" s="1"/>
+    </row>
+    <row r="384" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J384" s="1"/>
+      <c r="K384" s="1"/>
+    </row>
+    <row r="385" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J385" s="1"/>
+      <c r="K385" s="1"/>
+    </row>
+    <row r="386" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J386" s="1"/>
+      <c r="K386" s="1"/>
+    </row>
+    <row r="387" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J387" s="1"/>
+      <c r="K387" s="1"/>
+    </row>
+    <row r="388" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J388" s="1"/>
+      <c r="K388" s="1"/>
+    </row>
+    <row r="389" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J389" s="1"/>
+      <c r="K389" s="1"/>
+    </row>
+    <row r="390" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J390" s="1"/>
+      <c r="K390" s="1"/>
+    </row>
+    <row r="391" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J391" s="1"/>
+      <c r="K391" s="1"/>
+    </row>
+    <row r="392" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J392" s="1"/>
+      <c r="K392" s="1"/>
+    </row>
+    <row r="393" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J393" s="1"/>
+      <c r="K393" s="1"/>
+    </row>
+    <row r="394" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J394" s="1"/>
+      <c r="K394" s="1"/>
+    </row>
+    <row r="395" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J395" s="1"/>
+      <c r="K395" s="1"/>
+    </row>
+    <row r="396" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J396" s="1"/>
+      <c r="K396" s="1"/>
+    </row>
+    <row r="397" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J397" s="1"/>
+      <c r="K397" s="1"/>
+    </row>
+    <row r="398" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J398" s="1"/>
+      <c r="K398" s="1"/>
+    </row>
+    <row r="399" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J399" s="1"/>
+      <c r="K399" s="1"/>
+    </row>
+    <row r="400" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J400" s="1"/>
+      <c r="K400" s="1"/>
+    </row>
+    <row r="401" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J401" s="1"/>
+      <c r="K401" s="1"/>
+    </row>
+    <row r="402" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J402" s="1"/>
+      <c r="K402" s="1"/>
+    </row>
+    <row r="403" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J403" s="1"/>
+      <c r="K403" s="1"/>
+    </row>
+    <row r="404" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J404" s="1"/>
+      <c r="K404" s="1"/>
+    </row>
+    <row r="405" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J405" s="1"/>
+      <c r="K405" s="1"/>
+    </row>
+    <row r="406" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J406" s="1"/>
+      <c r="K406" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added round 4 bids
</commit_message>
<xml_diff>
--- a/database/seeds/numbers.xlsx
+++ b/database/seeds/numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn/Documents/NUS/Hackers/eusoff/database/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AA1385-B88F-C542-8984-D515003B3502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A182BA-6461-0F43-91E9-6F9832AF9938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36740" yWindow="1240" windowWidth="26160" windowHeight="16140" xr2:uid="{FC1533EE-1F79-D746-81F8-7CD84BC7FDEF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
 </sst>
 </file>
@@ -415,8 +412,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I406"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,7 +793,7 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
@@ -812,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -848,7 +845,7 @@
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
@@ -877,7 +874,7 @@
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -900,7 +897,7 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E37" t="s">
         <v>5</v>
@@ -913,7 +910,7 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
         <v>5</v>
@@ -926,7 +923,7 @@
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
         <v>5</v>
@@ -952,7 +949,7 @@
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E41" t="s">
         <v>5</v>
@@ -1033,7 +1030,7 @@
         <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -1056,10 +1053,10 @@
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1069,10 +1066,10 @@
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -1098,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -1108,10 +1105,10 @@
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -1121,7 +1118,7 @@
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E54" t="s">
         <v>5</v>
@@ -1134,10 +1131,10 @@
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -1160,10 +1157,10 @@
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -1176,7 +1173,7 @@
         <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -1189,7 +1186,7 @@
         <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -1199,10 +1196,10 @@
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -1212,10 +1209,10 @@
         <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -1225,10 +1222,10 @@
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -1238,7 +1235,7 @@
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E63" t="s">
         <v>5</v>
@@ -1251,10 +1248,10 @@
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -1277,7 +1274,7 @@
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
         <v>5</v>
@@ -1290,7 +1287,7 @@
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E67" t="s">
         <v>5</v>
@@ -1303,7 +1300,7 @@
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E68" t="s">
         <v>5</v>
@@ -1316,10 +1313,10 @@
         <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -1332,7 +1329,7 @@
         <v>5</v>
       </c>
       <c r="E70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -1342,7 +1339,7 @@
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" t="s">
         <v>5</v>
@@ -1358,7 +1355,7 @@
         <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -1368,7 +1365,7 @@
         <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E73" t="s">
         <v>5</v>
@@ -1381,10 +1378,10 @@
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
@@ -1394,7 +1391,7 @@
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E75" t="s">
         <v>5</v>
@@ -1410,7 +1407,7 @@
         <v>5</v>
       </c>
       <c r="E76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
@@ -1420,10 +1417,10 @@
         <v>76</v>
       </c>
       <c r="D77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
@@ -1433,7 +1430,7 @@
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E78" t="s">
         <v>5</v>
@@ -1446,7 +1443,7 @@
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E79" t="s">
         <v>5</v>
@@ -1462,7 +1459,7 @@
         <v>5</v>
       </c>
       <c r="E80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
@@ -1485,10 +1482,10 @@
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
@@ -1498,10 +1495,10 @@
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
@@ -1511,10 +1508,10 @@
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -1527,7 +1524,7 @@
         <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -1537,10 +1534,10 @@
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E86" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -1550,10 +1547,10 @@
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -1566,7 +1563,7 @@
         <v>5</v>
       </c>
       <c r="E88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -1589,10 +1586,10 @@
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -1602,10 +1599,10 @@
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -1615,7 +1612,7 @@
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E92" t="s">
         <v>5</v>
@@ -1628,7 +1625,7 @@
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E93" t="s">
         <v>5</v>
@@ -1641,10 +1638,10 @@
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
@@ -1654,7 +1651,7 @@
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E95" t="s">
         <v>5</v>
@@ -1667,7 +1664,7 @@
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E96" t="s">
         <v>5</v>
@@ -1696,7 +1693,7 @@
         <v>5</v>
       </c>
       <c r="E98" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
@@ -1709,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="E99" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>

</xml_diff>